<commit_message>
Refactor statement generation examples and enhance configuration handling: streamline demo scripts to utilize in-memory configurations, improve Excel export functionality, and ensure consistent formatting and linting across all modified files.
</commit_message>
<xml_diff>
--- a/examples/scripts/output/financial_statements.xlsx/income_statement.xlsx
+++ b/examples/scripts/output/financial_statements.xlsx/income_statement.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -581,376 +581,6 @@
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Research &amp; Development</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>r_d</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>-100</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>-120</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>-130</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>-137</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>-158</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Selling, General &amp; Administrative</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>sg_a</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>-200</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>-250</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>-239</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>-251</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>-243</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Depreciation &amp; Amortization</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>depreciation_amortization</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>-30</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>-35</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>-36</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>-37</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>-38</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Total Operating Expenses</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>total_operating_expenses</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>330</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>405</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>405</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>426</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>439</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  EBITDA</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>ebitda</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1,700</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2,070</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2,314</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2,622</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>2,975</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Operating Income (EBIT)</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>operating_income</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1,070</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>1,295</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>1,540</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>1,808</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>2,134</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Interest Expense</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>interest_expense</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>-50</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>-60</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>-63</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>-66</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>-69</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Earnings Before Tax</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>ebt</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1,120</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>1,355</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>1,603</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>1,874</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>2,204</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Income Tax Expense</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>taxes</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>-75</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>-90</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>-108</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>-130</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>-156</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Net Income</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>net_income</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>1,195</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>1,445</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>1,711</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>2,003</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>2,359</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>